<commit_message>
revisione con dati tbm corretti, grafici con testi leggibili, utilizzo main thrust force anziché auxiliary
</commit_message>
<xml_diff>
--- a/resources/tbm.xlsx
+++ b/resources/tbm.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual" refMode="R1C1"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -455,9 +455,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Foglio1"/>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -745,7 +747,7 @@
         <v>5.04</v>
       </c>
       <c r="I4" s="1">
-        <v>5.04</v>
+        <v>5.13</v>
       </c>
       <c r="J4" s="1">
         <v>7.0000000000000007E-2</v>
@@ -783,7 +785,7 @@
         <v>3500</v>
       </c>
       <c r="U4" s="1">
-        <v>13700</v>
+        <v>17700</v>
       </c>
       <c r="V4" s="1">
         <v>23266</v>
@@ -793,6 +795,36 @@
       </c>
       <c r="X4" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f>J2+(I2-H2)/2</f>
+        <v>7.9999999999999599E-2</v>
+      </c>
+      <c r="K7">
+        <f>2*J7</f>
+        <v>0.1599999999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f>J3+(I3-H3)/2</f>
+        <v>8.0000000000000016E-2</v>
+      </c>
+      <c r="K8">
+        <f>2*J8</f>
+        <v>0.16000000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f>J4+(I4-H4)/2</f>
+        <v>0.11499999999999994</v>
+      </c>
+      <c r="K9">
+        <f>2*J9</f>
+        <v>0.22999999999999987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>